<commit_message>
Make edits to schedule
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -5,15 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hyosubkim/Documents/GitHub/intro-to-programming/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hyosubkim/Documents/GitHub/datasci-for-kin/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B23B6138-C143-6042-9E15-DBE2919BB60C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED19B074-8811-1A40-AFDF-1E231A46C9A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="260" yWindow="760" windowWidth="22920" windowHeight="18880" xr2:uid="{3B080A87-D3C3-A64C-8B1B-295ED2108A51}"/>
+    <workbookView xWindow="30240" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="2" xr2:uid="{3B080A87-D3C3-A64C-8B1B-295ED2108A51}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="121">
   <si>
     <t>Date</t>
   </si>
@@ -57,9 +59,6 @@
   </si>
   <si>
     <t>Lab 4</t>
-  </si>
-  <si>
-    <t>Lect 5</t>
   </si>
   <si>
     <t>Lab 5</t>
@@ -515,10 +514,103 @@
     <t>Thanksgiving</t>
   </si>
   <si>
-    <t>10/12/2023 (Makeup Monday)</t>
-  </si>
-  <si>
     <t>Remeberance Day (Observation)</t>
+  </si>
+  <si>
+    <t>Lect 5 (Make-up Monday)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Organizational meeting, Meet and Greet, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>"about-this-course.ipynb"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>; Talk about chapter reading. Getting started - tech stack ("intro-to-jupyter-and-syzygy")</t>
+    </r>
+  </si>
+  <si>
+    <t>Read syllabus, 'about-this-course', 'what-is-datacience' ; A0-intro.ipynb. Reading (Nature article); download assignment from JupyterHub, complete, and upload it.</t>
+  </si>
+  <si>
+    <t>Lab0_jupyter-and-syzygy; lab1-var-assignment.ipynb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quiz 1; writing_a_function.ipynb </t>
+  </si>
+  <si>
+    <t>Lecture</t>
+  </si>
+  <si>
+    <t>Lab</t>
+  </si>
+  <si>
+    <t>Midterm Exam</t>
+  </si>
+  <si>
+    <t>Single Unit Data &amp; Spike Trains</t>
+  </si>
+  <si>
+    <t>Topic</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Learn about the tech stack used in this course, espcially how Jupyter notebooks work.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Introduction to Python </t>
+  </si>
+  <si>
+    <t>Learn about variables and assignment, converting variable types.</t>
+  </si>
+  <si>
+    <t>Python built-ins, lists, and dictionaries</t>
+  </si>
+  <si>
+    <t>Learn about Python functions and two key Python types, lists and dictionaries.</t>
+  </si>
+  <si>
+    <t>Flow control</t>
+  </si>
+  <si>
+    <t>Introduction to this course</t>
+  </si>
+  <si>
+    <t>Learn about loops and conditional ("if-then") statements.</t>
+  </si>
+  <si>
+    <t>Quiz 1</t>
+  </si>
+  <si>
+    <t>Covers concepts from weeks 1-4</t>
+  </si>
+  <si>
+    <t>Functions</t>
+  </si>
+  <si>
+    <t>Learn how to write your own custom functions.</t>
+  </si>
+  <si>
+    <t>Functions (cont'd)</t>
+  </si>
+  <si>
+    <t>More review and practice with functions.</t>
   </si>
 </sst>
 </file>
@@ -627,7 +719,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -689,6 +781,18 @@
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1006,8 +1110,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38F75CE4-F56E-AD47-A7ED-5AF26A01A21F}">
   <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1022,13 +1126,13 @@
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D1" s="12" t="s">
         <v>1</v>
@@ -1037,7 +1141,7 @@
         <v>2</v>
       </c>
       <c r="F1" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="85" x14ac:dyDescent="0.2">
@@ -1048,16 +1152,16 @@
         <v>45175</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E2" s="19" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="51" x14ac:dyDescent="0.2">
@@ -1068,16 +1172,16 @@
         <v>45180</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -1088,14 +1192,14 @@
         <v>45182</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E4" s="9"/>
       <c r="F4" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="68" x14ac:dyDescent="0.2">
@@ -1106,16 +1210,16 @@
         <v>45187</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -1126,10 +1230,10 @@
         <v>45189</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E6" s="9"/>
       <c r="F6" s="10"/>
@@ -1145,13 +1249,13 @@
         <v>3</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -1165,11 +1269,11 @@
         <v>4</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E8" s="10"/>
       <c r="F8" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="102" x14ac:dyDescent="0.2">
@@ -1180,7 +1284,7 @@
         <v>45201</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D9" s="15"/>
       <c r="E9" s="10"/>
@@ -1197,13 +1301,13 @@
         <v>5</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E10" s="16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -1214,7 +1318,7 @@
         <v>45208</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D11" s="16"/>
       <c r="E11" s="16"/>
@@ -1231,29 +1335,29 @@
         <v>6</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E12" s="10"/>
       <c r="F12" s="10"/>
     </row>
-    <row r="13" spans="1:6" ht="68" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A13" s="7">
         <v>6</v>
       </c>
-      <c r="B13" s="21" t="s">
+      <c r="B13" s="21">
+        <v>45211</v>
+      </c>
+      <c r="C13" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="C13" s="10" t="s">
-        <v>7</v>
-      </c>
       <c r="D13" s="15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E13" s="15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -1264,14 +1368,14 @@
         <v>45215</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E14" s="10"/>
       <c r="F14" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="136" x14ac:dyDescent="0.2">
@@ -1282,16 +1386,16 @@
         <v>45217</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E15" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -1302,10 +1406,10 @@
         <v>45222</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
@@ -1318,16 +1422,16 @@
         <v>45224</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D17" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E17" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="F17" s="10" t="s">
         <v>21</v>
-      </c>
-      <c r="E17" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="F17" s="10" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -1338,10 +1442,10 @@
         <v>45229</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
@@ -1354,16 +1458,16 @@
         <v>45231</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D19" s="16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E19" s="15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F19" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -1374,10 +1478,10 @@
         <v>45236</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D20" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E20" s="10"/>
       <c r="F20" s="10"/>
@@ -1390,13 +1494,13 @@
         <v>45238</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F21" s="10"/>
     </row>
@@ -1408,14 +1512,14 @@
         <v>45243</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D22" s="12"/>
       <c r="E22" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F22" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -1426,7 +1530,7 @@
         <v>45245</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D23" s="12"/>
       <c r="E23" s="12"/>
@@ -1440,16 +1544,16 @@
         <v>45250</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E24" s="16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F24" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -1460,10 +1564,10 @@
         <v>45252</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D25" s="15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E25" s="8"/>
       <c r="F25" s="8"/>
@@ -1476,16 +1580,16 @@
         <v>45257</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D26" s="15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E26" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F26" s="10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -1496,14 +1600,14 @@
         <v>45259</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D27" s="18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E27" s="10"/>
       <c r="F27" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="51" x14ac:dyDescent="0.2">
@@ -1514,14 +1618,14 @@
         <v>45264</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D28" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E28" s="10"/>
       <c r="F28" s="10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -1532,10 +1636,10 @@
         <v>45266</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D29" s="15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E29" s="10"/>
       <c r="F29" s="10"/>
@@ -1546,10 +1650,10 @@
       </c>
       <c r="B30" s="7"/>
       <c r="C30" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E30" s="10"/>
       <c r="F30" s="10"/>
@@ -1568,47 +1672,797 @@
       </c>
       <c r="B32" s="7"/>
       <c r="C32" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D32" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E32" s="10"/>
       <c r="F32" s="10"/>
     </row>
     <row r="35" spans="4:6" ht="34" x14ac:dyDescent="0.2">
       <c r="D35" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="37" spans="4:6" ht="68" x14ac:dyDescent="0.2">
       <c r="D37" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F37" s="17" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="38" spans="4:6" ht="34" x14ac:dyDescent="0.2">
       <c r="D38" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="39" spans="4:6" ht="17" x14ac:dyDescent="0.2">
       <c r="D39" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="40" spans="4:6" ht="17" x14ac:dyDescent="0.2">
       <c r="D40" s="14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D086929D-3C8C-5A48-93DB-9EAF3D41E809}">
+  <dimension ref="A1:F40"/>
+  <sheetViews>
+    <sheetView topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="7" style="6" customWidth="1"/>
+    <col min="2" max="2" width="9.1640625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="13.83203125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="45" style="2" customWidth="1"/>
+    <col min="5" max="5" width="37.33203125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="41.33203125" style="2" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="85" x14ac:dyDescent="0.2">
+      <c r="A2" s="7">
+        <v>1</v>
+      </c>
+      <c r="B2" s="20">
+        <v>45175</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="E2" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="A3" s="7">
+        <v>2</v>
+      </c>
+      <c r="B3" s="20">
+        <v>45180</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="7">
+        <v>2</v>
+      </c>
+      <c r="B4" s="20">
+        <v>45182</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="E4" s="9"/>
+      <c r="F4" s="10" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="68" x14ac:dyDescent="0.2">
+      <c r="A5" s="7">
+        <v>3</v>
+      </c>
+      <c r="B5" s="20">
+        <v>45187</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="7">
+        <v>3</v>
+      </c>
+      <c r="B6" s="20">
+        <v>45189</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="E6" s="9"/>
+      <c r="F6" s="10"/>
+    </row>
+    <row r="7" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="A7" s="7">
+        <v>4</v>
+      </c>
+      <c r="B7" s="20">
+        <v>45194</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="E7" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A8" s="7">
+        <v>4</v>
+      </c>
+      <c r="B8" s="20">
+        <v>45196</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="68" x14ac:dyDescent="0.2">
+      <c r="A9" s="7">
+        <v>5</v>
+      </c>
+      <c r="B9" s="20">
+        <v>45201</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="D9" s="15"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+    </row>
+    <row r="10" spans="1:6" ht="68" x14ac:dyDescent="0.2">
+      <c r="A10" s="7">
+        <v>5</v>
+      </c>
+      <c r="B10" s="20">
+        <v>45203</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A11" s="7">
+        <v>6</v>
+      </c>
+      <c r="B11" s="20">
+        <v>45208</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+    </row>
+    <row r="12" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A12" s="7">
+        <v>6</v>
+      </c>
+      <c r="B12" s="20">
+        <v>45210</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+    </row>
+    <row r="13" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="A13" s="7">
+        <v>6</v>
+      </c>
+      <c r="B13" s="21">
+        <v>45211</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A14" s="7">
+        <v>7</v>
+      </c>
+      <c r="B14" s="20">
+        <v>45215</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="136" x14ac:dyDescent="0.2">
+      <c r="A15" s="7">
+        <v>7</v>
+      </c>
+      <c r="B15" s="20">
+        <v>45217</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A16" s="7">
+        <v>8</v>
+      </c>
+      <c r="B16" s="20">
+        <v>45222</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="D16" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E16" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="F16" s="10"/>
+    </row>
+    <row r="17" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="A17" s="7">
+        <v>8</v>
+      </c>
+      <c r="B17" s="20">
+        <v>45224</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="D17" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="F17" s="10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A18" s="7">
+        <v>9</v>
+      </c>
+      <c r="B18" s="20">
+        <v>45229</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="D18" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="E18" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="F18" s="10"/>
+    </row>
+    <row r="19" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A19" s="7">
+        <v>9</v>
+      </c>
+      <c r="B19" s="20">
+        <v>45231</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="F19" s="10" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="A20" s="7">
+        <v>10</v>
+      </c>
+      <c r="B20" s="20">
+        <v>45236</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="E20" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="F20" s="10"/>
+    </row>
+    <row r="21" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A21" s="7">
+        <v>10</v>
+      </c>
+      <c r="B21" s="20">
+        <v>45238</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="D21" s="22" t="s">
+        <v>103</v>
+      </c>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
+    </row>
+    <row r="22" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="A22" s="7">
+        <v>11</v>
+      </c>
+      <c r="B22" s="20">
+        <v>45243</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="F22" s="12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A23" s="7">
+        <v>11</v>
+      </c>
+      <c r="B23" s="20">
+        <v>45245</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
+    </row>
+    <row r="24" spans="1:6" ht="153" x14ac:dyDescent="0.2">
+      <c r="A24" s="7">
+        <v>12</v>
+      </c>
+      <c r="B24" s="20">
+        <v>45250</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D24" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="F24" s="10" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A25" s="7">
+        <v>12</v>
+      </c>
+      <c r="B25" s="20">
+        <v>45252</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D25" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="E25" s="8"/>
+      <c r="F25" s="8"/>
+    </row>
+    <row r="26" spans="1:6" ht="102" x14ac:dyDescent="0.2">
+      <c r="A26" s="7">
+        <v>13</v>
+      </c>
+      <c r="B26" s="20">
+        <v>45257</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D26" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="E26" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="F26" s="10" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A27" s="7">
+        <v>13</v>
+      </c>
+      <c r="B27" s="20">
+        <v>45259</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D27" s="23" t="s">
+        <v>104</v>
+      </c>
+      <c r="E27" s="10"/>
+      <c r="F27" s="10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="A28" s="7">
+        <v>14</v>
+      </c>
+      <c r="B28" s="20">
+        <v>45264</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D28" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="E28" s="10"/>
+      <c r="F28" s="10" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A29" s="7">
+        <v>14</v>
+      </c>
+      <c r="B29" s="20">
+        <v>45266</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D29" s="15"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="10"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" s="7"/>
+      <c r="B30" s="7"/>
+      <c r="C30" s="10"/>
+      <c r="D30" s="10"/>
+      <c r="E30" s="10"/>
+      <c r="F30" s="10"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" s="7"/>
+      <c r="B31" s="7"/>
+      <c r="C31" s="10"/>
+      <c r="D31" s="10"/>
+      <c r="E31" s="10"/>
+      <c r="F31" s="10"/>
+    </row>
+    <row r="32" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A32" s="7">
+        <v>15</v>
+      </c>
+      <c r="B32" s="7"/>
+      <c r="C32" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D32" s="10"/>
+      <c r="E32" s="10"/>
+      <c r="F32" s="10"/>
+    </row>
+    <row r="35" spans="4:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="D35" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="37" spans="4:6" ht="68" x14ac:dyDescent="0.2">
+      <c r="D37" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F37" s="17" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="38" spans="4:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="D38" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="39" spans="4:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="D39" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="40" spans="4:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="D40" s="14" t="s">
+        <v>67</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7423716E-0C94-BF47-8EE7-34B4B9E97256}">
+  <dimension ref="A1:C16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="2"/>
+    <col min="2" max="2" width="24.1640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="42" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="17" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="C1" s="24" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A2" s="25">
+        <v>1</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>113</v>
+      </c>
+      <c r="C2" s="25" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A3" s="25">
+        <v>2</v>
+      </c>
+      <c r="B3" s="25" t="s">
+        <v>108</v>
+      </c>
+      <c r="C3" s="25" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A4" s="25">
+        <v>3</v>
+      </c>
+      <c r="B4" s="25" t="s">
+        <v>110</v>
+      </c>
+      <c r="C4" s="25" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A5" s="25">
+        <v>4</v>
+      </c>
+      <c r="B5" s="25" t="s">
+        <v>112</v>
+      </c>
+      <c r="C5" s="25" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="25">
+        <v>5</v>
+      </c>
+      <c r="B6" s="25" t="s">
+        <v>115</v>
+      </c>
+      <c r="C6" s="25" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" s="2">
+        <v>5</v>
+      </c>
+      <c r="B7" s="25" t="s">
+        <v>117</v>
+      </c>
+      <c r="C7" s="25" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A8" s="25">
+        <v>6</v>
+      </c>
+      <c r="B8" s="25" t="s">
+        <v>119</v>
+      </c>
+      <c r="C8" s="25" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="25">
+        <v>7</v>
+      </c>
+      <c r="B9" s="25"/>
+      <c r="C9" s="25"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="25">
+        <v>8</v>
+      </c>
+      <c r="B10" s="25"/>
+      <c r="C10" s="25"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="25">
+        <v>9</v>
+      </c>
+      <c r="B11" s="25"/>
+      <c r="C11" s="25"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="25">
+        <v>10</v>
+      </c>
+      <c r="B12" s="25"/>
+      <c r="C12" s="25"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="25">
+        <v>11</v>
+      </c>
+      <c r="B13" s="25"/>
+      <c r="C13" s="25"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="25">
+        <v>12</v>
+      </c>
+      <c r="B14" s="25"/>
+      <c r="C14" s="25"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="25">
+        <v>13</v>
+      </c>
+      <c r="B15" s="25"/>
+      <c r="C15" s="25"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="25">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Make edits to syllabus and preamble
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hyosubkim/Documents/GitHub/datasci-for-kin/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C669A8D-1F8F-DE4D-81CC-F6F102875AA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F752D040-C0B4-E64F-8167-1AE0101A788C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30900" yWindow="540" windowWidth="16720" windowHeight="20620" activeTab="2" xr2:uid="{3B080A87-D3C3-A64C-8B1B-295ED2108A51}"/>
+    <workbookView xWindow="35200" yWindow="500" windowWidth="26680" windowHeight="20120" activeTab="1" xr2:uid="{3B080A87-D3C3-A64C-8B1B-295ED2108A51}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1769,7 +1769,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D086929D-3C8C-5A48-93DB-9EAF3D41E809}">
   <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
       <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
@@ -2356,7 +2356,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7423716E-0C94-BF47-8EE7-34B4B9E97256}">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Clean up jupyter intro nb to use in lecture
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hyosubkim/Documents/GitHub/datasci-for-kin/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F752D040-C0B4-E64F-8167-1AE0101A788C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE81D306-561E-074A-8F74-996F491A336D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35200" yWindow="500" windowWidth="26680" windowHeight="20120" activeTab="1" xr2:uid="{3B080A87-D3C3-A64C-8B1B-295ED2108A51}"/>
+    <workbookView xWindow="1320" yWindow="880" windowWidth="26680" windowHeight="18880" activeTab="1" xr2:uid="{3B080A87-D3C3-A64C-8B1B-295ED2108A51}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -520,6 +520,123 @@
     <t>Lect 5 (Make-up Monday)</t>
   </si>
   <si>
+    <t>Lab0_jupyter-and-syzygy; lab1-var-assignment.ipynb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quiz 1; writing_a_function.ipynb </t>
+  </si>
+  <si>
+    <t>Lecture</t>
+  </si>
+  <si>
+    <t>Lab</t>
+  </si>
+  <si>
+    <t>Midterm Exam</t>
+  </si>
+  <si>
+    <t>Single Unit Data &amp; Spike Trains</t>
+  </si>
+  <si>
+    <t>Topic</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Learn about the tech stack used in this course, espcially how Jupyter notebooks work.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Introduction to Python </t>
+  </si>
+  <si>
+    <t>Learn about variables and assignment, converting variable types.</t>
+  </si>
+  <si>
+    <t>Python built-ins, lists, and dictionaries</t>
+  </si>
+  <si>
+    <t>Learn about Python functions and two key Python types, lists and dictionaries.</t>
+  </si>
+  <si>
+    <t>Flow control</t>
+  </si>
+  <si>
+    <t>Introduction to this course</t>
+  </si>
+  <si>
+    <t>Learn about loops and conditional ("if-then") statements.</t>
+  </si>
+  <si>
+    <t>Quiz 1</t>
+  </si>
+  <si>
+    <t>Covers concepts from weeks 1-4</t>
+  </si>
+  <si>
+    <t>Functions</t>
+  </si>
+  <si>
+    <t>Learn how to write your own custom functions.</t>
+  </si>
+  <si>
+    <t>Functions (cont'd)</t>
+  </si>
+  <si>
+    <t>More review and practice with functions.</t>
+  </si>
+  <si>
+    <t>6 (Make-up)</t>
+  </si>
+  <si>
+    <t>NumPy lecutre and lab; lab5_numpy (based on A5 from Gribble course)</t>
+  </si>
+  <si>
+    <t>Pandas lab; Subplots and lab7_matplotlib.ipynb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">data_cleaning.ipynb (may want to revise some parts of the outlier section); </t>
+  </si>
+  <si>
+    <t>signal processing lab</t>
+  </si>
+  <si>
+    <t>extra stuff, like conda installation, git, terminal, etc.</t>
+  </si>
+  <si>
+    <t>File I/O and Pandas</t>
+  </si>
+  <si>
+    <t>More visualization with seaborn</t>
+  </si>
+  <si>
+    <t>Intro to Exploratory Data Analysis and Repeated Measures</t>
+  </si>
+  <si>
+    <t>Data cleaning and dealing with outliers</t>
+  </si>
+  <si>
+    <t>Basic stats with Python</t>
+  </si>
+  <si>
+    <t>Remembrance Day and Midterm Break</t>
+  </si>
+  <si>
+    <t>Single Unit Data &amp; Spike Trains, and numerical computing with NumPy</t>
+  </si>
+  <si>
+    <t>Extras: Anaconda installation, git, terminal, etc.</t>
+  </si>
+  <si>
+    <t>make-up time</t>
+  </si>
+  <si>
+    <t>Data visualization with Matplotlib</t>
+  </si>
+  <si>
+    <t>Read syllabus, Textbook chapters "About this course" and "Intro to Data Science" ; A0-intro.ipynb. Reading (Nature article); download assignment from JupyterHub, complete, and upload it.</t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">Organizational meeting, Meet and Greet, </t>
     </r>
@@ -540,125 +657,8 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>; Talk about chapter reading. Getting started - tech stack ("intro-to-jupyter-and-syzygy")</t>
+      <t>; Slides generated from 1st two chapters; Getting started - tech stack (students follow along and type within "jupyter-jhub-student" notebook)</t>
     </r>
-  </si>
-  <si>
-    <t>Read syllabus, 'about-this-course', 'what-is-datacience' ; A0-intro.ipynb. Reading (Nature article); download assignment from JupyterHub, complete, and upload it.</t>
-  </si>
-  <si>
-    <t>Lab0_jupyter-and-syzygy; lab1-var-assignment.ipynb</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Quiz 1; writing_a_function.ipynb </t>
-  </si>
-  <si>
-    <t>Lecture</t>
-  </si>
-  <si>
-    <t>Lab</t>
-  </si>
-  <si>
-    <t>Midterm Exam</t>
-  </si>
-  <si>
-    <t>Single Unit Data &amp; Spike Trains</t>
-  </si>
-  <si>
-    <t>Topic</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Learn about the tech stack used in this course, espcially how Jupyter notebooks work.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Introduction to Python </t>
-  </si>
-  <si>
-    <t>Learn about variables and assignment, converting variable types.</t>
-  </si>
-  <si>
-    <t>Python built-ins, lists, and dictionaries</t>
-  </si>
-  <si>
-    <t>Learn about Python functions and two key Python types, lists and dictionaries.</t>
-  </si>
-  <si>
-    <t>Flow control</t>
-  </si>
-  <si>
-    <t>Introduction to this course</t>
-  </si>
-  <si>
-    <t>Learn about loops and conditional ("if-then") statements.</t>
-  </si>
-  <si>
-    <t>Quiz 1</t>
-  </si>
-  <si>
-    <t>Covers concepts from weeks 1-4</t>
-  </si>
-  <si>
-    <t>Functions</t>
-  </si>
-  <si>
-    <t>Learn how to write your own custom functions.</t>
-  </si>
-  <si>
-    <t>Functions (cont'd)</t>
-  </si>
-  <si>
-    <t>More review and practice with functions.</t>
-  </si>
-  <si>
-    <t>6 (Make-up)</t>
-  </si>
-  <si>
-    <t>NumPy lecutre and lab; lab5_numpy (based on A5 from Gribble course)</t>
-  </si>
-  <si>
-    <t>Pandas lab; Subplots and lab7_matplotlib.ipynb</t>
-  </si>
-  <si>
-    <t xml:space="preserve">data_cleaning.ipynb (may want to revise some parts of the outlier section); </t>
-  </si>
-  <si>
-    <t>signal processing lab</t>
-  </si>
-  <si>
-    <t>extra stuff, like conda installation, git, terminal, etc.</t>
-  </si>
-  <si>
-    <t>File I/O and Pandas</t>
-  </si>
-  <si>
-    <t>More visualization with seaborn</t>
-  </si>
-  <si>
-    <t>Intro to Exploratory Data Analysis and Repeated Measures</t>
-  </si>
-  <si>
-    <t>Data cleaning and dealing with outliers</t>
-  </si>
-  <si>
-    <t>Basic stats with Python</t>
-  </si>
-  <si>
-    <t>Remembrance Day and Midterm Break</t>
-  </si>
-  <si>
-    <t>Single Unit Data &amp; Spike Trains, and numerical computing with NumPy</t>
-  </si>
-  <si>
-    <t>Extras: Anaconda installation, git, terminal, etc.</t>
-  </si>
-  <si>
-    <t>make-up time</t>
-  </si>
-  <si>
-    <t>Data visualization with Matplotlib</t>
   </si>
 </sst>
 </file>
@@ -1769,8 +1769,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D086929D-3C8C-5A48-93DB-9EAF3D41E809}">
   <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1814,10 +1814,10 @@
         <v>36</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>97</v>
+        <v>136</v>
       </c>
       <c r="E2" s="19" t="s">
-        <v>98</v>
+        <v>135</v>
       </c>
       <c r="F2" s="10" t="s">
         <v>65</v>
@@ -1854,7 +1854,7 @@
         <v>38</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E4" s="9"/>
       <c r="F4" s="10" t="s">
@@ -1960,7 +1960,7 @@
         <v>5</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E10" s="15" t="s">
         <v>51</v>
@@ -2026,7 +2026,7 @@
         <v>45215</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D14" s="16" t="s">
         <v>23</v>
@@ -2046,10 +2046,10 @@
         <v>45217</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F15" s="10" t="s">
         <v>88</v>
@@ -2063,7 +2063,7 @@
         <v>45222</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D16" s="9" t="s">
         <v>71</v>
@@ -2081,7 +2081,7 @@
         <v>45224</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D17" s="15"/>
       <c r="F17" s="10" t="s">
@@ -2096,7 +2096,7 @@
         <v>45229</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D18" s="15" t="s">
         <v>16</v>
@@ -2111,10 +2111,10 @@
         <v>45231</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F19" s="10" t="s">
         <v>69</v>
@@ -2128,7 +2128,7 @@
         <v>45236</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>46</v>
@@ -2143,10 +2143,10 @@
         <v>45238</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D21" s="22" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E21" s="10"/>
       <c r="F21" s="10"/>
@@ -2192,7 +2192,7 @@
         <v>26</v>
       </c>
       <c r="D24" s="23" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E24" s="13" t="s">
         <v>52</v>
@@ -2212,7 +2212,7 @@
         <v>27</v>
       </c>
       <c r="D25" s="14" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E25" s="10"/>
       <c r="F25" s="8"/>
@@ -2245,7 +2245,7 @@
         <v>29</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E27" s="10"/>
       <c r="F27" s="10" t="s">
@@ -2263,7 +2263,7 @@
         <v>30</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F28" s="10" t="s">
         <v>75</v>
@@ -2280,7 +2280,7 @@
         <v>31</v>
       </c>
       <c r="D29" s="13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E29" s="10"/>
       <c r="F29" s="10"/>
@@ -2373,10 +2373,10 @@
         <v>41</v>
       </c>
       <c r="B1" s="24" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C1" s="24" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -2384,10 +2384,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C2" s="25" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -2395,10 +2395,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="25" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C3" s="25" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -2406,10 +2406,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -2417,10 +2417,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="25" t="s">
+        <v>110</v>
+      </c>
+      <c r="C5" s="25" t="s">
         <v>112</v>
-      </c>
-      <c r="C5" s="25" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -2428,10 +2428,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -2439,10 +2439,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="25" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C7" s="25" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -2450,18 +2450,18 @@
         <v>6</v>
       </c>
       <c r="B8" s="25" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C8" s="25" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B9" s="25" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C9" s="25"/>
     </row>
@@ -2470,7 +2470,7 @@
         <v>7</v>
       </c>
       <c r="B10" s="25" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C10" s="25"/>
     </row>
@@ -2486,7 +2486,7 @@
         <v>8</v>
       </c>
       <c r="B12" s="25" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C12" s="25"/>
     </row>
@@ -2495,7 +2495,7 @@
         <v>9</v>
       </c>
       <c r="B13" s="25" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C13" s="25"/>
     </row>
@@ -2504,7 +2504,7 @@
         <v>9</v>
       </c>
       <c r="B14" s="25" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C14" s="25"/>
     </row>
@@ -2513,7 +2513,7 @@
         <v>10</v>
       </c>
       <c r="B15" s="25" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C15" s="25"/>
     </row>
@@ -2522,7 +2522,7 @@
         <v>10</v>
       </c>
       <c r="B16" s="25" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C16" s="25"/>
     </row>
@@ -2531,7 +2531,7 @@
         <v>11</v>
       </c>
       <c r="B17" s="25" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C17" s="25"/>
     </row>
@@ -2540,7 +2540,7 @@
         <v>12</v>
       </c>
       <c r="B18" s="25" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C18" s="25"/>
     </row>
@@ -2557,7 +2557,7 @@
         <v>14</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Edit sched and latex eqn in nb
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hyosubkim/Documents/GitHub/datasci-for-kin/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DAF5D14-E967-D54C-B936-A6948F4CB105}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A02BAD4C-79B7-3644-865E-A48251B992DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="34700" yWindow="900" windowWidth="26680" windowHeight="18880" xr2:uid="{3B080A87-D3C3-A64C-8B1B-295ED2108A51}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="117">
   <si>
     <t>Date</t>
   </si>
@@ -162,13 +162,7 @@
     <t>Complete RM data tutorial (leave code out of student notebooks and text)</t>
   </si>
   <si>
-    <t xml:space="preserve">Only for this lecture, go through intro nb together. Make sure everyone knows how to work technology. Also, add figs to intro nb. </t>
-  </si>
-  <si>
     <t>A1-data-types-expressions.ipynb</t>
-  </si>
-  <si>
-    <t>Consider adding evaluating expressions.</t>
   </si>
   <si>
     <t xml:space="preserve">Check out "fortyforloops.ipynb" from NYU course in tutorials folder - may be good lecture or lab material. Consider removing info on lambda functions from lecture. </t>
@@ -995,7 +989,7 @@
   <dimension ref="A1:G40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1017,7 +1011,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D1" s="10" t="s">
         <v>1</v>
@@ -1026,10 +1020,10 @@
         <v>2</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="102" x14ac:dyDescent="0.2">
@@ -1043,17 +1037,17 @@
         <v>26</v>
       </c>
       <c r="D2" s="21" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E2" s="24" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F2" s="24"/>
       <c r="G2" s="21" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="19">
         <v>2</v>
       </c>
@@ -1064,17 +1058,15 @@
         <v>27</v>
       </c>
       <c r="D3" s="21" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E3" s="21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F3" s="21" t="s">
-        <v>110</v>
-      </c>
-      <c r="G3" s="21" t="s">
-        <v>41</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="G3" s="21"/>
     </row>
     <row r="4" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="19">
@@ -1087,13 +1079,11 @@
         <v>28</v>
       </c>
       <c r="D4" s="21" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E4" s="21"/>
       <c r="F4" s="21"/>
-      <c r="G4" s="21" t="s">
-        <v>43</v>
-      </c>
+      <c r="G4" s="21"/>
     </row>
     <row r="5" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A5" s="19">
@@ -1106,14 +1096,14 @@
         <v>29</v>
       </c>
       <c r="D5" s="21" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E5" s="21" t="s">
         <v>15</v>
       </c>
       <c r="F5" s="21"/>
       <c r="G5" s="21" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -1127,11 +1117,11 @@
         <v>30</v>
       </c>
       <c r="D6" s="21" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E6" s="21"/>
       <c r="F6" s="21" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="G6" s="21"/>
     </row>
@@ -1146,16 +1136,16 @@
         <v>3</v>
       </c>
       <c r="D7" s="24" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E7" s="24" t="s">
         <v>35</v>
       </c>
       <c r="F7" s="24" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G7" s="21" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="34" x14ac:dyDescent="0.2">
@@ -1169,12 +1159,12 @@
         <v>4</v>
       </c>
       <c r="D8" s="21" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E8" s="21"/>
       <c r="F8" s="21"/>
       <c r="G8" s="21" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="68" x14ac:dyDescent="0.2">
@@ -1185,7 +1175,7 @@
         <v>45201</v>
       </c>
       <c r="C9" s="21" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D9" s="21"/>
       <c r="E9" s="21"/>
@@ -1203,14 +1193,14 @@
         <v>5</v>
       </c>
       <c r="D10" s="21" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E10" s="21" t="s">
         <v>36</v>
       </c>
       <c r="F10" s="21"/>
       <c r="G10" s="21" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -1221,7 +1211,7 @@
         <v>45208</v>
       </c>
       <c r="C11" s="21" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D11" s="22"/>
       <c r="E11" s="21"/>
@@ -1239,7 +1229,7 @@
         <v>6</v>
       </c>
       <c r="D12" s="21" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E12" s="21"/>
       <c r="F12" s="21"/>
@@ -1253,7 +1243,7 @@
         <v>45211</v>
       </c>
       <c r="C13" s="21" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D13" s="21" t="s">
         <v>13</v>
@@ -1262,10 +1252,10 @@
         <v>38</v>
       </c>
       <c r="F13" s="21" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G13" s="21" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="34" x14ac:dyDescent="0.2">
@@ -1276,7 +1266,7 @@
         <v>45215</v>
       </c>
       <c r="C14" s="21" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D14" s="24" t="s">
         <v>16</v>
@@ -1285,10 +1275,10 @@
         <v>39</v>
       </c>
       <c r="F14" s="21" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G14" s="21" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="136" x14ac:dyDescent="0.2">
@@ -1302,12 +1292,12 @@
         <v>7</v>
       </c>
       <c r="D15" s="21" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E15" s="22"/>
       <c r="F15" s="22"/>
       <c r="G15" s="21" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="51" x14ac:dyDescent="0.2">
@@ -1318,10 +1308,10 @@
         <v>45222</v>
       </c>
       <c r="C16" s="21" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D16" s="21" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E16" s="24" t="s">
         <v>40</v>
@@ -1354,14 +1344,14 @@
         <v>45229</v>
       </c>
       <c r="C18" s="21" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D18" s="21" t="s">
         <v>12</v>
       </c>
       <c r="E18" s="22"/>
       <c r="F18" s="22" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="G18" s="21"/>
     </row>
@@ -1376,12 +1366,12 @@
         <v>9</v>
       </c>
       <c r="D19" s="21" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E19" s="22"/>
       <c r="F19" s="22"/>
       <c r="G19" s="21" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -1392,7 +1382,7 @@
         <v>45236</v>
       </c>
       <c r="C20" s="21" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D20" s="22" t="s">
         <v>33</v>
@@ -1412,7 +1402,7 @@
         <v>10</v>
       </c>
       <c r="D21" s="24" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E21" s="21"/>
       <c r="F21" s="21"/>
@@ -1426,7 +1416,7 @@
         <v>45243</v>
       </c>
       <c r="C22" s="21" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D22" s="21"/>
       <c r="E22" s="21" t="s">
@@ -1463,14 +1453,14 @@
         <v>18</v>
       </c>
       <c r="D24" s="22" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E24" s="21" t="s">
         <v>37</v>
       </c>
       <c r="F24" s="21"/>
       <c r="G24" s="21" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="34" x14ac:dyDescent="0.2">
@@ -1481,10 +1471,10 @@
         <v>45252</v>
       </c>
       <c r="C25" s="21" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D25" s="22" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E25" s="21"/>
       <c r="F25" s="21"/>
@@ -1506,7 +1496,7 @@
       <c r="E26" s="22"/>
       <c r="F26" s="22"/>
       <c r="G26" s="21" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="34" x14ac:dyDescent="0.2">
@@ -1520,7 +1510,7 @@
         <v>19</v>
       </c>
       <c r="D27" s="17" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E27" s="8"/>
       <c r="F27" s="8"/>
@@ -1539,10 +1529,10 @@
         <v>22</v>
       </c>
       <c r="D28" s="17" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G28" s="8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -1556,7 +1546,7 @@
         <v>21</v>
       </c>
       <c r="D29" s="18" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E29" s="8"/>
       <c r="F29" s="8"/>
@@ -1643,10 +1633,10 @@
         <v>31</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -1654,10 +1644,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -1665,10 +1655,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -1676,10 +1666,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -1687,10 +1677,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="C5" s="16" t="s">
         <v>71</v>
-      </c>
-      <c r="C5" s="16" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1698,10 +1688,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1709,10 +1699,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1720,18 +1710,18 @@
         <v>6</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C9" s="16"/>
     </row>
@@ -1740,7 +1730,7 @@
         <v>7</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C10" s="16"/>
     </row>
@@ -1756,7 +1746,7 @@
         <v>8</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C12" s="16"/>
     </row>
@@ -1765,7 +1755,7 @@
         <v>9</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C13" s="16"/>
     </row>
@@ -1774,7 +1764,7 @@
         <v>9</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C14" s="16"/>
     </row>
@@ -1783,7 +1773,7 @@
         <v>10</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C15" s="16"/>
     </row>
@@ -1792,7 +1782,7 @@
         <v>10</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C16" s="16"/>
     </row>
@@ -1801,7 +1791,7 @@
         <v>11</v>
       </c>
       <c r="B17" s="16" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C17" s="16"/>
     </row>
@@ -1810,7 +1800,7 @@
         <v>12</v>
       </c>
       <c r="B18" s="16" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C18" s="16"/>
     </row>
@@ -1827,7 +1817,7 @@
         <v>14</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Clean up RM nb
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hyosubkim/Documents/GitHub/datasci-for-kin/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01B1CE93-DFBC-924D-AC3D-5068E29F993D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EA71291-D8A2-1B41-8896-F599335DF21B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34700" yWindow="900" windowWidth="26680" windowHeight="18880" xr2:uid="{3B080A87-D3C3-A64C-8B1B-295ED2108A51}"/>
+    <workbookView xWindow="35580" yWindow="1300" windowWidth="26680" windowHeight="18880" xr2:uid="{3B080A87-D3C3-A64C-8B1B-295ED2108A51}"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="116">
   <si>
     <t>Date</t>
   </si>
@@ -72,9 +72,6 @@
     <t>Lab 8</t>
   </si>
   <si>
-    <t>Looping over data files</t>
-  </si>
-  <si>
     <t>Intro to EDA and RM data</t>
   </si>
   <si>
@@ -90,9 +87,6 @@
     <t>Data visualization with Matplotlib; Procedural versus OOP in Matplotlib</t>
   </si>
   <si>
-    <t xml:space="preserve">This is more advanced material that would normally come right after pandas lecture. </t>
-  </si>
-  <si>
     <t>Lect 10</t>
   </si>
   <si>
@@ -153,12 +147,6 @@
     <t>A5-numpy-assignment.ipynb</t>
   </si>
   <si>
-    <t>A6-pandas-assignment.ipynb</t>
-  </si>
-  <si>
-    <t>A7-matplotlib.ipynb</t>
-  </si>
-  <si>
     <t>Complete RM data tutorial (leave code out of student notebooks and text)</t>
   </si>
   <si>
@@ -171,9 +159,6 @@
     <t>Consider beefing up the lab a little.</t>
   </si>
   <si>
-    <t>Lecture and lab nbs need minor editorial clean-up (e.g., creating drop-downs for solutions). Use dynamical systems example in lecture.</t>
-  </si>
-  <si>
     <t>For lecture, go through Exercises in plotting,ipynb.</t>
   </si>
   <si>
@@ -268,9 +253,6 @@
   </si>
   <si>
     <t>6 (Make-up)</t>
-  </si>
-  <si>
-    <t>Pandas lab; Subplots and lab7_matplotlib.ipynb</t>
   </si>
   <si>
     <t xml:space="preserve">data_cleaning.ipynb (may want to revise some parts of the outlier section); </t>
@@ -479,14 +461,41 @@
     <t>lab1-jupyter-variables.ipynb</t>
   </si>
   <si>
+    <t>**Reminders:**</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The labs should have instructor and student versions, with and without solution. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">May want to rewrite answer to part 2 of simulating dynamical system. The indexing is a bit tricky. </t>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
         <sz val="12"/>
-        <color theme="1"/>
+        <color rgb="FFFF0000"/>
         <rFont val="Calibri (Body)"/>
       </rPr>
-      <t>Thinking about data for plotting (plotting_types.ipynb); seaborn.ipynb</t>
+      <t>Quiz 1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve">; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>writing_a_function.ipynb</t>
     </r>
     <r>
       <rPr>
@@ -499,42 +508,18 @@
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
+  </si>
+  <si>
+    <t>"Looping over data files" is more advanced? Should come right after pandas lecture. Could I make functions material shorter?</t>
+  </si>
+  <si>
     <r>
       <rPr>
-        <b/>
         <sz val="12"/>
         <color theme="1"/>
         <rFont val="Calibri (Body)"/>
       </rPr>
-      <t>and human_factors.ipynb</t>
-    </r>
-  </si>
-  <si>
-    <t>**Reminders:**</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The labs should have instructor and student versions, with and without solution. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">May want to rewrite answer to part 2 of simulating dynamical system. The indexing is a bit tricky. </t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t>Quiz 1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t xml:space="preserve">; </t>
+      <t>Thinking about data for plotting (plotting_types.ipynb); seaborn.ipynb</t>
     </r>
     <r>
       <rPr>
@@ -544,26 +529,38 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>writing_a_function.ipynb</t>
+      <t xml:space="preserve"> </t>
     </r>
     <r>
       <rPr>
-        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>and human_factors.ipynb</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
         <sz val="12"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
+      <t>Pandas lab; Subplots and lab7_matplotlib.ipynb</t>
+    </r>
+  </si>
+  <si>
+    <t>A5-pandas-and-matplotlib.ipynb</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -609,13 +606,6 @@
       <name val="Calibri (Body)"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FF00B0F0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="12"/>
       <color rgb="FFFF0000"/>
@@ -656,7 +646,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -704,41 +694,32 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1056,8 +1037,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D086929D-3C8C-5A48-93DB-9EAF3D41E809}">
   <dimension ref="A1:G40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1073,13 +1054,13 @@
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="D1" s="9" t="s">
         <v>1</v>
@@ -1088,10 +1069,10 @@
         <v>2</v>
       </c>
       <c r="F1" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="G1" s="9" t="s">
         <v>98</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="102" x14ac:dyDescent="0.2">
@@ -1102,17 +1083,17 @@
         <v>45175</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="E2" s="16" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="F2" s="16"/>
       <c r="G2" s="7" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -1123,16 +1104,16 @@
         <v>45180</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="G3" s="7"/>
     </row>
@@ -1144,10 +1125,10 @@
         <v>45182</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
@@ -1161,17 +1142,17 @@
         <v>45187</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="E5" s="17" t="s">
-        <v>15</v>
+        <v>97</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>14</v>
       </c>
       <c r="F5" s="7"/>
       <c r="G5" s="7" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -1182,14 +1163,14 @@
         <v>45189</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="E6" s="7"/>
       <c r="F6" s="7" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="G6" s="7"/>
     </row>
@@ -1204,13 +1185,13 @@
         <v>3</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="E7" s="18" t="s">
-        <v>35</v>
+        <v>46</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>33</v>
       </c>
       <c r="F7" s="16" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="G7" s="7"/>
     </row>
@@ -1225,12 +1206,12 @@
         <v>4</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
       <c r="G8" s="7" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="68" x14ac:dyDescent="0.2">
@@ -1241,7 +1222,7 @@
         <v>45201</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="D9" s="7"/>
       <c r="E9" s="7"/>
@@ -1252,32 +1233,32 @@
       <c r="A10" s="8">
         <v>5</v>
       </c>
-      <c r="B10" s="19">
+      <c r="B10" s="17">
         <v>45203</v>
       </c>
       <c r="C10" s="9" t="s">
         <v>5</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>118</v>
-      </c>
-      <c r="E10" s="9" t="s">
-        <v>36</v>
+        <v>111</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>34</v>
       </c>
       <c r="F10" s="9"/>
       <c r="G10" s="9" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="8">
         <v>6</v>
       </c>
-      <c r="B11" s="19">
+      <c r="B11" s="17">
         <v>45208</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D11" s="12"/>
       <c r="E11" s="9"/>
@@ -1288,110 +1269,106 @@
       <c r="A12" s="8">
         <v>6</v>
       </c>
-      <c r="B12" s="19">
+      <c r="B12" s="17">
         <v>45210</v>
       </c>
       <c r="C12" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="27" t="s">
-        <v>50</v>
+      <c r="D12" s="7" t="s">
+        <v>45</v>
       </c>
       <c r="E12" s="9"/>
       <c r="F12" s="9"/>
       <c r="G12" s="9" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" s="8">
         <v>6</v>
       </c>
-      <c r="B13" s="20">
+      <c r="B13" s="18">
         <v>45211</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="E13" s="9" t="s">
-        <v>38</v>
+        <v>52</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" s="25" t="s">
+        <v>115</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="G13" s="9" t="s">
-        <v>44</v>
-      </c>
+        <v>102</v>
+      </c>
+      <c r="G13" s="9"/>
     </row>
     <row r="14" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" s="8">
         <v>7</v>
       </c>
-      <c r="B14" s="19">
+      <c r="B14" s="17">
         <v>45215</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="D14" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="E14" s="9" t="s">
-        <v>39</v>
-      </c>
+        <v>87</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" s="9"/>
       <c r="F14" s="9" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="136" x14ac:dyDescent="0.2">
       <c r="A15" s="8">
         <v>7</v>
       </c>
-      <c r="B15" s="19">
+      <c r="B15" s="17">
         <v>45217</v>
       </c>
       <c r="C15" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D15" s="9" t="s">
-        <v>77</v>
+      <c r="D15" s="7" t="s">
+        <v>114</v>
       </c>
       <c r="E15" s="12"/>
       <c r="F15" s="12"/>
       <c r="G15" s="9" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="51" x14ac:dyDescent="0.2">
       <c r="A16" s="8">
         <v>8</v>
       </c>
-      <c r="B16" s="19">
+      <c r="B16" s="17">
         <v>45222</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="D16" s="9" t="s">
-        <v>114</v>
-      </c>
-      <c r="E16" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="F16" s="21"/>
+        <v>88</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="E16" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="F16" s="19"/>
       <c r="G16" s="9"/>
     </row>
     <row r="17" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A17" s="8">
         <v>8</v>
       </c>
-      <c r="B17" s="19">
+      <c r="B17" s="17">
         <v>45224</v>
       </c>
       <c r="C17" s="9" t="s">
@@ -1401,25 +1378,25 @@
       <c r="E17" s="12"/>
       <c r="F17" s="12"/>
       <c r="G17" s="9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="8">
         <v>9</v>
       </c>
-      <c r="B18" s="19">
+      <c r="B18" s="17">
         <v>45229</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E18" s="12"/>
       <c r="F18" s="12" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="G18" s="9"/>
     </row>
@@ -1427,33 +1404,33 @@
       <c r="A19" s="8">
         <v>9</v>
       </c>
-      <c r="B19" s="19">
+      <c r="B19" s="17">
         <v>45231</v>
       </c>
       <c r="C19" s="9" t="s">
         <v>9</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="E19" s="12"/>
       <c r="F19" s="12"/>
       <c r="G19" s="9" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="8">
         <v>10</v>
       </c>
-      <c r="B20" s="19">
+      <c r="B20" s="17">
         <v>45236</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E20" s="12"/>
       <c r="F20" s="12"/>
@@ -1463,14 +1440,14 @@
       <c r="A21" s="8">
         <v>10</v>
       </c>
-      <c r="B21" s="19">
+      <c r="B21" s="17">
         <v>45238</v>
       </c>
       <c r="C21" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D21" s="26" t="s">
-        <v>58</v>
+      <c r="D21" s="24" t="s">
+        <v>53</v>
       </c>
       <c r="E21" s="9"/>
       <c r="F21" s="9"/>
@@ -1480,30 +1457,30 @@
       <c r="A22" s="8">
         <v>11</v>
       </c>
-      <c r="B22" s="19">
+      <c r="B22" s="17">
         <v>45243</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D22" s="9"/>
       <c r="E22" s="9" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F22" s="9"/>
       <c r="G22" s="9" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="8">
         <v>11</v>
       </c>
-      <c r="B23" s="19">
+      <c r="B23" s="17">
         <v>45245</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D23" s="12"/>
       <c r="E23" s="12"/>
@@ -1514,109 +1491,109 @@
       <c r="A24" s="8">
         <v>12</v>
       </c>
-      <c r="B24" s="19">
+      <c r="B24" s="17">
         <v>45250</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D24" s="12" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="E24" s="9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F24" s="9"/>
       <c r="G24" s="9" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A25" s="8">
         <v>12</v>
       </c>
-      <c r="B25" s="19">
+      <c r="B25" s="17">
         <v>45252</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="E25" s="9"/>
       <c r="F25" s="9"/>
-      <c r="G25" s="22"/>
+      <c r="G25" s="20"/>
     </row>
     <row r="26" spans="1:7" ht="102" x14ac:dyDescent="0.2">
       <c r="A26" s="8">
         <v>13</v>
       </c>
-      <c r="B26" s="19">
+      <c r="B26" s="17">
         <v>45257</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E26" s="12"/>
       <c r="F26" s="12"/>
       <c r="G26" s="9" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A27" s="8">
         <v>13</v>
       </c>
-      <c r="B27" s="19">
+      <c r="B27" s="17">
         <v>45259</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="D27" s="23" t="s">
-        <v>79</v>
+        <v>17</v>
+      </c>
+      <c r="D27" s="21" t="s">
+        <v>73</v>
       </c>
       <c r="E27" s="9"/>
       <c r="F27" s="9"/>
       <c r="G27" s="9" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A28" s="8">
         <v>14</v>
       </c>
-      <c r="B28" s="19">
+      <c r="B28" s="17">
         <v>45264</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D28" s="23" t="s">
-        <v>80</v>
+        <v>20</v>
+      </c>
+      <c r="D28" s="21" t="s">
+        <v>74</v>
       </c>
       <c r="E28" s="12"/>
       <c r="F28" s="12"/>
       <c r="G28" s="9" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="8">
         <v>14</v>
       </c>
-      <c r="B29" s="19">
+      <c r="B29" s="17">
         <v>45266</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="D29" s="24" t="s">
-        <v>89</v>
+        <v>19</v>
+      </c>
+      <c r="D29" s="22" t="s">
+        <v>83</v>
       </c>
       <c r="E29" s="9"/>
       <c r="F29" s="9"/>
@@ -1646,7 +1623,7 @@
       </c>
       <c r="B32" s="8"/>
       <c r="C32" s="9" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D32" s="9"/>
       <c r="E32" s="9"/>
@@ -1654,8 +1631,8 @@
       <c r="G32" s="9"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A33" s="25"/>
-      <c r="B33" s="25"/>
+      <c r="A33" s="23"/>
+      <c r="B33" s="23"/>
       <c r="C33" s="12"/>
       <c r="D33" s="12"/>
       <c r="E33" s="12"/>
@@ -1663,40 +1640,38 @@
       <c r="G33" s="12"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A34" s="25"/>
-      <c r="B34" s="25"/>
+      <c r="A34" s="23"/>
+      <c r="B34" s="23"/>
       <c r="C34" s="12"/>
       <c r="D34" s="11"/>
       <c r="E34" s="12"/>
       <c r="F34" s="12"/>
       <c r="G34" s="12"/>
     </row>
-    <row r="35" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A35" s="25"/>
-      <c r="B35" s="25"/>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A35" s="23"/>
+      <c r="B35" s="23"/>
       <c r="C35" s="12"/>
-      <c r="D35" s="12" t="s">
-        <v>11</v>
-      </c>
+      <c r="D35" s="12"/>
       <c r="E35" s="12"/>
       <c r="F35" s="12"/>
-      <c r="G35" s="12" t="s">
-        <v>17</v>
-      </c>
+      <c r="G35" s="12"/>
     </row>
     <row r="36" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="D36" s="28" t="s">
-        <v>115</v>
+      <c r="D36" s="2" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="D37" s="2" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="G37" s="12"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="D38" s="3"/>
+    <row r="38" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+      <c r="D38" s="3" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D39" s="4"/>
@@ -1727,13 +1702,13 @@
   <sheetData>
     <row r="1" spans="1:3" s="12" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="14" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -1741,10 +1716,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -1752,10 +1727,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -1763,10 +1738,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -1774,10 +1749,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1785,10 +1760,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1796,10 +1771,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1807,18 +1782,18 @@
         <v>6</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="C9" s="15"/>
     </row>
@@ -1827,7 +1802,7 @@
         <v>7</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="C10" s="15"/>
     </row>
@@ -1843,7 +1818,7 @@
         <v>8</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="C12" s="15"/>
     </row>
@@ -1852,7 +1827,7 @@
         <v>9</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C13" s="15"/>
     </row>
@@ -1861,7 +1836,7 @@
         <v>9</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="C14" s="15"/>
     </row>
@@ -1870,7 +1845,7 @@
         <v>10</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="C15" s="15"/>
     </row>
@@ -1879,7 +1854,7 @@
         <v>10</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C16" s="15"/>
     </row>
@@ -1888,7 +1863,7 @@
         <v>11</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="C17" s="15"/>
     </row>
@@ -1897,7 +1872,7 @@
         <v>12</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="C18" s="15"/>
     </row>
@@ -1906,7 +1881,7 @@
         <v>13</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="51" x14ac:dyDescent="0.2">
@@ -1914,7 +1889,7 @@
         <v>14</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>